<commit_message>
Updated the framework with env in a separate folder
</commit_message>
<xml_diff>
--- a/contentpaths.xlsx
+++ b/contentpaths.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,15 +412,12 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/de/de/basic-login/forgot-password</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Preview activated</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/podcast-examples</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/gr/el/build-test/el/tools-to-support-a-new-conversation/understand-the-impact-of-your-ad</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/tabs-test-page</v>
       </c>
       <c r="B3" t="str">
         <v>Preview activated</v>
@@ -428,7 +425,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/nl/nl/exzeem/tips-bij-eczeem</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/test-gif</v>
       </c>
       <c r="B4" t="str">
         <v>Preview activated</v>
@@ -436,7 +433,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/cz/cs/archive-cf/cs/pribehy-pacientu</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/test-logo-lozenge-combination</v>
       </c>
       <c r="B5" t="str">
         <v>Preview activated</v>
@@ -444,20 +441,20 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/fi/fi/set-password</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Preview activated</v>
+        <v>/content/abbvie-pro/uk/en/neuroscience/parkinsons/products/duodopa-what-is-apd/contact-us/abc</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/sa/en1/tools-to-support-a-new-conversation/planning-your-next-appointment/appointment-preparation-tool-short</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/test-aml-page</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Preview activated</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/basic-login/forgot-password</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/understanding-ndo</v>
       </c>
       <c r="B8" t="str">
         <v>Preview activated</v>
@@ -465,7 +462,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/at/de/blog/neurodermitis-stress-fuer-die-haut</v>
+        <v>/content/abbvie-pro/uk/en/neuroscience/migraine/aquipta/contact-us1/error</v>
       </c>
       <c r="B9" t="str">
         <v>Preview activated</v>
@@ -473,7 +470,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/jp/ja/facilities/Kinki</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/dosing-calculator</v>
       </c>
       <c r="B10" t="str">
         <v>Preview activated</v>
@@ -481,12 +478,39 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>/content/abbvie-lets-talk-eczema-ous/de/de/blog-beitraege/kunstaktion</v>
+        <v>/content/abbvie-pro/uk/en/test-podcast/test-header-and-footer-addition</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Preview activated</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>/content/abbvie-pro/uk/en/test-podcast/understanding-oab</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Preview activated</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>/content/abbvie-pro/uk/en/test-podcast/cll-life-test</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Preview activated</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>/content/abbvie-pro/uk/en/test-podcast/rinvoq-gastro-home-page-template</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Preview activated</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated script 16 Dec
</commit_message>
<xml_diff>
--- a/contentpaths.xlsx
+++ b/contentpaths.xlsx
@@ -1,41 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABBISH\Documents\Playwright\preview-activate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2CA59-5DF9-4423-A8D5-4605CB2E6A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29085" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Contents" sheetId="1" r:id="rId1"/>
+    <sheet name="Contents" sheetId="2" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Content Path</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>/content/abbvie-pro/de/de/therapy-areas/virology/hepatitis-c/service/thank-you-contact-request</t>
+  </si>
+  <si>
+    <t>/content/abbvie-pro/de/de/therapy-areas/oncology/hemato-oncology/artikel/closed/direct-downloads/eha23-tag1-cll2</t>
+  </si>
+  <si>
+    <t>/content/abbvie-pro/de/de/therapy-areas/oncology/hemato-oncology/artikel/closed/direct-downloads/kongresshighlights-ash-2022-t2-x1</t>
+  </si>
+  <si>
+    <t>/content/abbvie-pro/de/de/therapy-areas/immunology/dermatology/artikel/closed/fobi-kongressbericht-2024</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +74,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,119 +413,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F43F26-B351-4851-826A-A8F0F739176B}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="118.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Content Path</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>/content/allergan-pro-ami/ca/en/build-test/Welcome/Hematology/chronic-lymphocytic-leukemia</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Preview activated</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>/content/allergan-pro-ami/ca/fr/build-test/Bienvenue/Neurosciences/ChronicMigraine/PatientCaseStudy</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Preview activated</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>/content/allergan-pro-ami/ca/en/build-test/Welcome/gynecology/endometriosis</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Preview activated</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>/content/allergan-pro-ami/fr/fr/errors/403</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>/content/allergan-pro-ami/ca/en/Welcome/course-review</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>/content/allergan-pro-ami/ca/fr/build-test/Bienvenue/Neurosciences/SpasticityandMovementDisorders</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>/content/allergan-pro-ami/de/de/change-password</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>/content/allergan-pro-ami/fr/fr/event-page/remote-management</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>/content/allergan-pro-ami/ca/en/event-page/event-four</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>/content/allergan-pro-ami/ca/en/basic-login</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>/content/allergan-pro-ami/ca/en/event-page/event-2</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Preview activated</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>/content/allergan-pro-ami/ca/en/chronic-migraine</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Preview activated</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B13"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>